<commit_message>
save rats and preds
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="158">
   <si>
     <t xml:space="preserve">t1</t>
   </si>
@@ -63,6 +63,9 @@
     <t xml:space="preserve">44 8</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">20 38</t>
   </si>
   <si>
@@ -75,7 +78,7 @@
     <t xml:space="preserve">30 22</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
+    <t xml:space="preserve">46 12</t>
   </si>
   <si>
     <t xml:space="preserve">62 24</t>
@@ -90,12 +93,18 @@
     <t xml:space="preserve">16 28</t>
   </si>
   <si>
+    <t xml:space="preserve">36 22</t>
+  </si>
+  <si>
     <t xml:space="preserve">44 18</t>
   </si>
   <si>
     <t xml:space="preserve">40 0</t>
   </si>
   <si>
+    <t xml:space="preserve">36 12</t>
+  </si>
+  <si>
     <t xml:space="preserve">18 26</t>
   </si>
   <si>
@@ -120,6 +129,9 @@
     <t xml:space="preserve">24 26</t>
   </si>
   <si>
+    <t xml:space="preserve">34 20</t>
+  </si>
+  <si>
     <t xml:space="preserve">50 16</t>
   </si>
   <si>
@@ -183,6 +195,9 @@
     <t xml:space="preserve">27 26</t>
   </si>
   <si>
+    <t xml:space="preserve">31 12</t>
+  </si>
+  <si>
     <t xml:space="preserve">37 18</t>
   </si>
   <si>
@@ -460,6 +475,9 @@
   </si>
   <si>
     <t xml:space="preserve">22 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 20</t>
   </si>
   <si>
     <t xml:space="preserve">38 14</t>
@@ -586,10 +604,10 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -636,19 +654,25 @@
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,13 +680,13 @@
         <v>3</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,13 +694,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,7 +709,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="H6" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -694,24 +718,30 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>17</v>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,29 +749,32 @@
         <v>7</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>28</v>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,13 +782,13 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -777,10 +810,10 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.52"/>
@@ -803,275 +836,296 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1093,267 +1147,285 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>17</v>
+        <v>150</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>